<commit_message>
actualizando nombre de archivos
</commit_message>
<xml_diff>
--- a/Proyecto final.xlsx
+++ b/Proyecto final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johnny Jimenez\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UCREATIVA\I cuatri\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{9C49BBB8-CB57-4E66-A53B-CE2D41B5239C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DDD2FE2-8010-4243-A2C0-C671DDCA0922}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1E3445-B2D6-4D45-9AE4-256FC1800BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-2730" windowWidth="29040" windowHeight="15840" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -171,7 +171,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,12 +187,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -208,15 +214,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
@@ -552,11 +559,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33F345D-29AF-46DF-8449-AA46405E0794}">
   <dimension ref="B8:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="76.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.85546875" bestFit="1" customWidth="1"/>
@@ -570,82 +577,82 @@
     <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="8" spans="2:2">
-      <c r="B8" t="s">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:2">
-      <c r="B9" t="s">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:2">
-      <c r="B10" t="s">
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:2">
-      <c r="B11" t="s">
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="2:2">
-      <c r="B12" t="s">
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:2">
-      <c r="B13" t="s">
+    <row r="13" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:2">
-      <c r="B14" t="s">
+    <row r="14" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="2:2">
-      <c r="B15" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:2">
-      <c r="B16" t="s">
+    <row r="16" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="2:3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="25" spans="2:3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="2:3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="30" spans="2:3">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="31" spans="2:3">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>15</v>
       </c>
@@ -653,7 +660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="2:3">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>16</v>
       </c>
@@ -661,7 +668,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="33" spans="2:16">
+    <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>17</v>
       </c>
@@ -669,7 +676,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="2:16">
+    <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>18</v>
       </c>
@@ -677,12 +684,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:16">
+    <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="40" spans="2:16">
+    <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>20</v>
       </c>
@@ -693,7 +700,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="41" spans="2:16">
+    <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E41" t="s">
         <v>22</v>
       </c>
@@ -701,7 +708,7 @@
         <v>1250</v>
       </c>
     </row>
-    <row r="42" spans="2:16">
+    <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>23</v>
       </c>
@@ -712,7 +719,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="2:16">
+    <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>25</v>
       </c>
@@ -733,7 +740,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="44" spans="2:16">
+    <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E44" t="s">
         <v>27</v>
       </c>
@@ -762,7 +769,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="45" spans="2:16">
+    <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="E45" t="s">
         <v>33</v>
       </c>
@@ -802,7 +809,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="46" spans="2:16">
+    <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J46">
         <v>6</v>
       </c>
@@ -831,7 +838,7 @@
         <v>2208</v>
       </c>
     </row>
-    <row r="47" spans="2:16">
+    <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>34</v>
       </c>
@@ -866,7 +873,7 @@
         <v>2576</v>
       </c>
     </row>
-    <row r="48" spans="2:16">
+    <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>35</v>
       </c>
@@ -905,7 +912,7 @@
         <v>2944</v>
       </c>
     </row>
-    <row r="49" spans="2:16">
+    <row r="49" spans="2:16" x14ac:dyDescent="0.25">
       <c r="F49" s="1">
         <f>+F48/F43</f>
         <v>0.67605633802816911</v>
@@ -938,7 +945,7 @@
         <v>3312</v>
       </c>
     </row>
-    <row r="50" spans="2:16">
+    <row r="50" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J50">
         <v>10</v>
       </c>
@@ -967,12 +974,12 @@
         <v>3680</v>
       </c>
     </row>
-    <row r="52" spans="2:16">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
       <c r="G52" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="2:16">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>37</v>
       </c>
@@ -981,12 +988,12 @@
         <v>0.17605633802816911</v>
       </c>
     </row>
-    <row r="54" spans="2:16">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="55" spans="2:16">
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>39</v>
       </c>
@@ -994,7 +1001,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="2:16">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>41</v>
       </c>
@@ -1011,7 +1018,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="57" spans="2:16">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J57" t="s">
         <v>29</v>
       </c>
@@ -1031,7 +1038,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="2:16">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J58">
         <v>5</v>
       </c>
@@ -1060,7 +1067,7 @@
         <v>3135.7746478873241</v>
       </c>
     </row>
-    <row r="59" spans="2:16">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J59">
         <v>6</v>
       </c>
@@ -1089,7 +1096,7 @@
         <v>3762.929577464789</v>
       </c>
     </row>
-    <row r="60" spans="2:16">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J60">
         <v>7</v>
       </c>
@@ -1118,7 +1125,7 @@
         <v>4390.0845070422538</v>
       </c>
     </row>
-    <row r="61" spans="2:16">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J61">
         <v>8</v>
       </c>
@@ -1147,7 +1154,7 @@
         <v>5017.2394366197186</v>
       </c>
     </row>
-    <row r="62" spans="2:16">
+    <row r="62" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J62">
         <v>9</v>
       </c>
@@ -1176,7 +1183,7 @@
         <v>5644.3943661971834</v>
       </c>
     </row>
-    <row r="63" spans="2:16">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
       <c r="J63">
         <v>10</v>
       </c>
@@ -1205,7 +1212,7 @@
         <v>6271.5492957746483</v>
       </c>
     </row>
-    <row r="65" spans="2:16">
+    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>42</v>
       </c>
@@ -1213,42 +1220,42 @@
         <v>122.66670000000001</v>
       </c>
     </row>
-    <row r="68" spans="2:16">
+    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
     </row>
-    <row r="70" spans="2:16">
+    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
     </row>
-    <row r="71" spans="2:16">
+    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
     </row>
-    <row r="72" spans="2:16">
+    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
     </row>
-    <row r="73" spans="2:16">
+    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
     </row>
-    <row r="74" spans="2:16">
+    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
     </row>
-    <row r="75" spans="2:16">
+    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>

</xml_diff>

<commit_message>
actualizando avanze del excel
</commit_message>
<xml_diff>
--- a/Proyecto final.xlsx
+++ b/Proyecto final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UCREATIVA\I cuatri\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D1E3445-B2D6-4D45-9AE4-256FC1800BF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B931CD46-36D6-4310-AEAC-8FB9B7B3862F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
+    <workbookView xWindow="-14505" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="48">
   <si>
     <t>Datos a ingresar</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Formulas</t>
   </si>
   <si>
-    <t>Total de deudas * 100 / salario promedio = % de eudeudamiento</t>
-  </si>
-  <si>
     <t>Riesgo</t>
   </si>
   <si>
@@ -164,7 +161,25 @@
     <t>Escribir 'El cliente no es sujeto de crédito debido a su nivel de endeudamiento alto.'</t>
   </si>
   <si>
-    <t>formula(1300,1250,1000,800)</t>
+    <t>Total de deudas / salario promedio = % de eudeudamiento</t>
+  </si>
+  <si>
+    <t>Esto va en Calculo endeudamiento</t>
+  </si>
+  <si>
+    <t>Ingreso de Datos</t>
+  </si>
+  <si>
+    <t>tipo de cliente</t>
+  </si>
+  <si>
+    <t>Informe de ingresos</t>
+  </si>
+  <si>
+    <t>deudas cliente</t>
+  </si>
+  <si>
+    <t>calculo de endeudamiento</t>
   </si>
 </sst>
 </file>
@@ -187,7 +202,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,6 +212,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,12 +235,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F33F345D-29AF-46DF-8449-AA46405E0794}">
-  <dimension ref="B8:P75"/>
+  <dimension ref="B7:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:B16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52:G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,6 +599,11 @@
     <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>0</v>
@@ -622,38 +649,48 @@
         <v>8</v>
       </c>
     </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="22" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="23" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="25" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="4" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="4" t="s">
         <v>13</v>
       </c>
     </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="B30" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="31" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C31">
@@ -661,7 +698,7 @@
       </c>
     </row>
     <row r="32" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B32" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="2">
@@ -669,7 +706,7 @@
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="B33" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C33" s="2">
@@ -677,7 +714,7 @@
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="B34" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C34" s="2">
@@ -689,8 +726,13 @@
         <v>19</v>
       </c>
     </row>
+    <row r="39" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>45</v>
+      </c>
+    </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="B40" s="4" t="s">
         <v>20</v>
       </c>
       <c r="E40" t="s">
@@ -709,6 +751,9 @@
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>46</v>
+      </c>
       <c r="E42" t="s">
         <v>23</v>
       </c>
@@ -720,7 +765,7 @@
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="B43" s="4" t="s">
         <v>25</v>
       </c>
       <c r="E43" t="s">
@@ -810,6 +855,9 @@
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>47</v>
+      </c>
       <c r="J46">
         <v>6</v>
       </c>
@@ -839,7 +887,7 @@
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="B47" s="4" t="s">
         <v>34</v>
       </c>
       <c r="H47" t="s">
@@ -874,8 +922,8 @@
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>35</v>
+      <c r="B48" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="F48">
         <f>F44</f>
@@ -975,13 +1023,16 @@
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>42</v>
+      </c>
       <c r="G52" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B53" s="5" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>37</v>
       </c>
       <c r="G53" s="1">
         <f>+F49-0.5</f>
@@ -989,21 +1040,21 @@
       </c>
     </row>
     <row r="54" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="B54" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B55" s="5" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="55" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="M55" t="s">
         <v>39</v>
       </c>
-      <c r="M55" t="s">
+    </row>
+    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B56" s="5" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
-        <v>41</v>
       </c>
       <c r="M56" s="1">
         <f>0.75-G53</f>
@@ -1212,50 +1263,42 @@
         <v>6271.5492957746483</v>
       </c>
     </row>
-    <row r="65" spans="2:16" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
-        <v>42</v>
-      </c>
-      <c r="C65">
-        <v>122.66670000000001</v>
-      </c>
-    </row>
-    <row r="68" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M68" s="1"/>
       <c r="N68" s="1"/>
       <c r="O68" s="1"/>
     </row>
-    <row r="70" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M70" s="3"/>
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
       <c r="P70" s="3"/>
     </row>
-    <row r="71" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M71" s="3"/>
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
       <c r="P71" s="3"/>
     </row>
-    <row r="72" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M72" s="3"/>
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
       <c r="P72" s="3"/>
     </row>
-    <row r="73" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M73" s="3"/>
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
       <c r="P73" s="3"/>
     </row>
-    <row r="74" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M74" s="3"/>
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
       <c r="P74" s="3"/>
     </row>
-    <row r="75" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="13:16" x14ac:dyDescent="0.25">
       <c r="M75" s="3"/>
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>

</xml_diff>

<commit_message>
Se actualiza Calculo de endeudamiento utilizando los modulos mejorados
</commit_message>
<xml_diff>
--- a/Proyecto final.xlsx
+++ b/Proyecto final.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UCREATIVA\I cuatri\ProyectoFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4312DBAA-0C8A-4DEC-AD87-9E1EDDD80A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320DBBED-1AF9-4787-8520-1AF3F3F205B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,14 +241,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,7 +588,7 @@
   <dimension ref="B7:P75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="H45" sqref="H45"/>
+      <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -687,7 +686,7 @@
       </c>
     </row>
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B29" s="6" t="s">
+      <c r="B29" t="s">
         <v>44</v>
       </c>
     </row>

</xml_diff>

<commit_message>
creando productos  y probando menu
</commit_message>
<xml_diff>
--- a/Proyecto final.xlsx
+++ b/Proyecto final.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\UCREATIVA\I cuatri\ProyectoFinal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/30b51c4ec5bb18ed/Escritorio/ModeloGestionCrediticia/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{320DBBED-1AF9-4787-8520-1AF3F3F205B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{320DBBED-1AF9-4787-8520-1AF3F3F205B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4A7AF554-A0D3-4716-A03A-C49191DFA04B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{05105159-61C4-406A-832E-F3FDA705B0BE}"/>
   </bookViews>
@@ -588,7 +588,7 @@
   <dimension ref="B7:P75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D37" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -745,7 +745,7 @@
         <v>21</v>
       </c>
       <c r="F40">
-        <v>1300</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
@@ -753,7 +753,7 @@
         <v>22</v>
       </c>
       <c r="F41">
-        <v>1250</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>23</v>
       </c>
       <c r="F42">
-        <v>1000</v>
+        <v>1680</v>
       </c>
       <c r="M42" t="s">
         <v>24</v>
@@ -779,7 +779,7 @@
       </c>
       <c r="F43">
         <f>AVERAGE(F40:F42)</f>
-        <v>1183.3333333333333</v>
+        <v>1693.3333333333333</v>
       </c>
       <c r="M43" s="2">
         <v>0.75</v>
@@ -826,11 +826,11 @@
       </c>
       <c r="F45">
         <f>+F43-F44</f>
-        <v>383.33333333333326</v>
+        <v>893.33333333333326</v>
       </c>
       <c r="H45">
         <f>+F45*0.32</f>
-        <v>122.66666666666664</v>
+        <v>285.86666666666667</v>
       </c>
       <c r="J45">
         <v>5</v>
@@ -841,23 +841,23 @@
       </c>
       <c r="L45">
         <f>+K45*$H$45</f>
-        <v>7359.9999999999982</v>
+        <v>17152</v>
       </c>
       <c r="M45">
         <f>+L45*0.75</f>
-        <v>5519.9999999999982</v>
+        <v>12864</v>
       </c>
       <c r="N45">
         <f>+L45*0.55</f>
-        <v>4047.9999999999995</v>
+        <v>9433.6</v>
       </c>
       <c r="O45">
         <f>+L45*0.4</f>
-        <v>2943.9999999999995</v>
+        <v>6860.8</v>
       </c>
       <c r="P45">
         <f>+L45-M45</f>
-        <v>1840</v>
+        <v>4288</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
@@ -873,23 +873,23 @@
       </c>
       <c r="L46">
         <f t="shared" ref="L46:L50" si="1">+K46*$H$45</f>
-        <v>8831.9999999999982</v>
+        <v>20582.400000000001</v>
       </c>
       <c r="M46">
         <f t="shared" ref="M46:M50" si="2">+L46*0.75</f>
-        <v>6623.9999999999982</v>
+        <v>15436.800000000001</v>
       </c>
       <c r="N46">
         <f t="shared" ref="N46:N50" si="3">+L46*0.55</f>
-        <v>4857.5999999999995</v>
+        <v>11320.320000000002</v>
       </c>
       <c r="O46">
         <f t="shared" ref="O46:O50" si="4">+L46*0.4</f>
-        <v>3532.7999999999993</v>
+        <v>8232.9600000000009</v>
       </c>
       <c r="P46">
         <f t="shared" ref="P46:P63" si="5">+L46-M46</f>
-        <v>2208</v>
+        <v>5145.6000000000004</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
@@ -908,23 +908,23 @@
       </c>
       <c r="L47">
         <f t="shared" si="1"/>
-        <v>10303.999999999998</v>
+        <v>24012.799999999999</v>
       </c>
       <c r="M47">
         <f t="shared" si="2"/>
-        <v>7727.9999999999982</v>
+        <v>18009.599999999999</v>
       </c>
       <c r="N47">
         <f t="shared" si="3"/>
-        <v>5667.2</v>
+        <v>13207.04</v>
       </c>
       <c r="O47">
         <f t="shared" si="4"/>
-        <v>4121.5999999999995</v>
+        <v>9605.1200000000008</v>
       </c>
       <c r="P47">
         <f t="shared" si="5"/>
-        <v>2576</v>
+        <v>6003.2000000000007</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
@@ -950,23 +950,23 @@
       </c>
       <c r="L48">
         <f t="shared" si="1"/>
-        <v>11775.999999999998</v>
+        <v>27443.200000000001</v>
       </c>
       <c r="M48">
         <f t="shared" si="2"/>
-        <v>8831.9999999999982</v>
+        <v>20582.400000000001</v>
       </c>
       <c r="N48">
         <f t="shared" si="3"/>
-        <v>6476.7999999999993</v>
+        <v>15093.760000000002</v>
       </c>
       <c r="O48">
         <f t="shared" si="4"/>
-        <v>4710.3999999999996</v>
+        <v>10977.28</v>
       </c>
       <c r="P48">
         <f t="shared" si="5"/>
-        <v>2944</v>
+        <v>6860.7999999999993</v>
       </c>
     </row>
     <row r="49" spans="2:16" x14ac:dyDescent="0.25">
@@ -975,7 +975,7 @@
       </c>
       <c r="F49" s="1">
         <f>+F48/F43</f>
-        <v>0.67605633802816911</v>
+        <v>0.47244094488188976</v>
       </c>
       <c r="J49">
         <v>9</v>
@@ -986,23 +986,23 @@
       </c>
       <c r="L49">
         <f t="shared" si="1"/>
-        <v>13247.999999999998</v>
+        <v>30873.600000000002</v>
       </c>
       <c r="M49">
         <f t="shared" si="2"/>
-        <v>9935.9999999999982</v>
+        <v>23155.200000000001</v>
       </c>
       <c r="N49">
         <f t="shared" si="3"/>
-        <v>7286.4</v>
+        <v>16980.480000000003</v>
       </c>
       <c r="O49">
         <f t="shared" si="4"/>
-        <v>5299.2</v>
+        <v>12349.440000000002</v>
       </c>
       <c r="P49">
         <f t="shared" si="5"/>
-        <v>3312</v>
+        <v>7718.4000000000015</v>
       </c>
     </row>
     <row r="50" spans="2:16" x14ac:dyDescent="0.25">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="F50" s="1">
         <f>+F49-0.5</f>
-        <v>0.17605633802816911</v>
+        <v>-2.7559055118110243E-2</v>
       </c>
       <c r="J50">
         <v>10</v>
@@ -1022,23 +1022,23 @@
       </c>
       <c r="L50">
         <f t="shared" si="1"/>
-        <v>14719.999999999996</v>
+        <v>34304</v>
       </c>
       <c r="M50">
         <f t="shared" si="2"/>
-        <v>11039.999999999996</v>
+        <v>25728</v>
       </c>
       <c r="N50">
         <f t="shared" si="3"/>
-        <v>8095.9999999999991</v>
+        <v>18867.2</v>
       </c>
       <c r="O50">
         <f t="shared" si="4"/>
-        <v>5887.9999999999991</v>
+        <v>13721.6</v>
       </c>
       <c r="P50">
         <f t="shared" si="5"/>
-        <v>3680</v>
+        <v>8576</v>
       </c>
     </row>
     <row r="52" spans="2:16" x14ac:dyDescent="0.25">
@@ -1070,7 +1070,7 @@
       </c>
       <c r="M56" s="1">
         <f>0.75-F50</f>
-        <v>0.57394366197183089</v>
+        <v>0.77755905511811019</v>
       </c>
       <c r="N56" s="1">
         <f>0.55-H49</f>
@@ -1111,23 +1111,23 @@
       </c>
       <c r="L58">
         <f>+L45</f>
-        <v>7359.9999999999982</v>
+        <v>17152</v>
       </c>
       <c r="M58" s="3">
         <f>+L58*M$56</f>
-        <v>4224.225352112674</v>
+        <v>13336.692913385827</v>
       </c>
       <c r="N58" s="3">
         <f>+L58*N$56</f>
-        <v>4047.9999999999995</v>
+        <v>9433.6</v>
       </c>
       <c r="O58" s="3">
         <f>+L58*O$56</f>
-        <v>2943.9999999999995</v>
+        <v>6860.8</v>
       </c>
       <c r="P58" s="3">
         <f t="shared" si="5"/>
-        <v>3135.7746478873241</v>
+        <v>3815.3070866141734</v>
       </c>
     </row>
     <row r="59" spans="2:16" x14ac:dyDescent="0.25">
@@ -1140,23 +1140,23 @@
       </c>
       <c r="L59">
         <f t="shared" ref="L59:L63" si="7">+L46</f>
-        <v>8831.9999999999982</v>
+        <v>20582.400000000001</v>
       </c>
       <c r="M59" s="3">
         <f t="shared" ref="M59:M62" si="8">+L59*M$56</f>
-        <v>5069.0704225352092</v>
+        <v>16004.031496062993</v>
       </c>
       <c r="N59" s="3">
         <f t="shared" ref="N59:N63" si="9">+L59*N$56</f>
-        <v>4857.5999999999995</v>
+        <v>11320.320000000002</v>
       </c>
       <c r="O59" s="3">
         <f t="shared" ref="O59:O63" si="10">+L59*O$56</f>
-        <v>3532.7999999999993</v>
+        <v>8232.9600000000009</v>
       </c>
       <c r="P59" s="3">
         <f t="shared" si="5"/>
-        <v>3762.929577464789</v>
+        <v>4578.3685039370084</v>
       </c>
     </row>
     <row r="60" spans="2:16" x14ac:dyDescent="0.25">
@@ -1169,23 +1169,23 @@
       </c>
       <c r="L60">
         <f t="shared" si="7"/>
-        <v>10303.999999999998</v>
+        <v>24012.799999999999</v>
       </c>
       <c r="M60" s="3">
         <f t="shared" si="8"/>
-        <v>5913.9154929577444</v>
+        <v>18671.370078740154</v>
       </c>
       <c r="N60" s="3">
         <f t="shared" si="9"/>
-        <v>5667.2</v>
+        <v>13207.04</v>
       </c>
       <c r="O60" s="3">
         <f t="shared" si="10"/>
-        <v>4121.5999999999995</v>
+        <v>9605.1200000000008</v>
       </c>
       <c r="P60" s="3">
         <f t="shared" si="5"/>
-        <v>4390.0845070422538</v>
+        <v>5341.4299212598453</v>
       </c>
     </row>
     <row r="61" spans="2:16" x14ac:dyDescent="0.25">
@@ -1198,23 +1198,23 @@
       </c>
       <c r="L61">
         <f t="shared" si="7"/>
-        <v>11775.999999999998</v>
+        <v>27443.200000000001</v>
       </c>
       <c r="M61" s="3">
         <f t="shared" si="8"/>
-        <v>6758.7605633802796</v>
+        <v>21338.70866141732</v>
       </c>
       <c r="N61" s="3">
         <f t="shared" si="9"/>
-        <v>6476.7999999999993</v>
+        <v>15093.760000000002</v>
       </c>
       <c r="O61" s="3">
         <f t="shared" si="10"/>
-        <v>4710.3999999999996</v>
+        <v>10977.28</v>
       </c>
       <c r="P61" s="3">
         <f t="shared" si="5"/>
-        <v>5017.2394366197186</v>
+        <v>6104.4913385826803</v>
       </c>
     </row>
     <row r="62" spans="2:16" x14ac:dyDescent="0.25">
@@ -1227,23 +1227,23 @@
       </c>
       <c r="L62">
         <f t="shared" si="7"/>
-        <v>13247.999999999998</v>
+        <v>30873.600000000002</v>
       </c>
       <c r="M62" s="3">
         <f t="shared" si="8"/>
-        <v>7603.6056338028147</v>
+        <v>24006.047244094487</v>
       </c>
       <c r="N62" s="3">
         <f t="shared" si="9"/>
-        <v>7286.4</v>
+        <v>16980.480000000003</v>
       </c>
       <c r="O62" s="3">
         <f t="shared" si="10"/>
-        <v>5299.2</v>
+        <v>12349.440000000002</v>
       </c>
       <c r="P62" s="3">
         <f t="shared" si="5"/>
-        <v>5644.3943661971834</v>
+        <v>6867.5527559055154</v>
       </c>
     </row>
     <row r="63" spans="2:16" x14ac:dyDescent="0.25">
@@ -1256,23 +1256,23 @@
       </c>
       <c r="L63">
         <f t="shared" si="7"/>
-        <v>14719.999999999996</v>
+        <v>34304</v>
       </c>
       <c r="M63" s="3">
         <f>+L63*M$56</f>
-        <v>8448.4507042253481</v>
+        <v>26673.385826771653</v>
       </c>
       <c r="N63" s="3">
         <f t="shared" si="9"/>
-        <v>8095.9999999999991</v>
+        <v>18867.2</v>
       </c>
       <c r="O63" s="3">
         <f t="shared" si="10"/>
-        <v>5887.9999999999991</v>
+        <v>13721.6</v>
       </c>
       <c r="P63" s="3">
         <f t="shared" si="5"/>
-        <v>6271.5492957746483</v>
+        <v>7630.6141732283468</v>
       </c>
     </row>
     <row r="68" spans="13:16" x14ac:dyDescent="0.25">

</xml_diff>